<commit_message>
Thêm file event (nhưng còn thiếu load vào list)
</commit_message>
<xml_diff>
--- a/Data/HackBrain1-6.xlsx
+++ b/Data/HackBrain1-6.xlsx
@@ -1484,7 +1484,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>44066</v>
+        <v>44059</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -1507,7 +1507,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="1">
-        <v>44067</v>
+        <v>44060</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -1527,7 +1527,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="1">
-        <v>44068</v>
+        <v>44061</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
@@ -1547,7 +1547,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="1">
-        <v>44069</v>
+        <v>44070</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -1567,7 +1567,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="1">
-        <v>44070</v>
+        <v>44071</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -1587,7 +1587,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="1">
-        <v>44071</v>
+        <v>44072</v>
       </c>
       <c r="E7" t="s">
         <v>31</v>
@@ -1607,7 +1607,7 @@
         <v>34</v>
       </c>
       <c r="C8" s="1">
-        <v>44066</v>
+        <v>44073</v>
       </c>
       <c r="E8" t="s">
         <v>35</v>
@@ -1627,7 +1627,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="1">
-        <v>44067</v>
+        <v>44074</v>
       </c>
       <c r="E9" t="s">
         <v>39</v>
@@ -1647,7 +1647,7 @@
         <v>43</v>
       </c>
       <c r="C10" s="1">
-        <v>44068</v>
+        <v>44075</v>
       </c>
       <c r="E10" t="s">
         <v>44</v>
@@ -1709,7 +1709,7 @@
         <v>53</v>
       </c>
       <c r="C14" s="1">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="F14" t="s">
         <v>40</v>
@@ -1793,7 +1793,7 @@
         <v>65</v>
       </c>
       <c r="C20" s="1">
-        <v>44066</v>
+        <v>44068</v>
       </c>
       <c r="F20" t="s">
         <v>16</v>

</xml_diff>